<commit_message>
allow for override case where item pack assignment is blank in custom form
</commit_message>
<xml_diff>
--- a/app/config/tables/ctp_delivery/forms/ctp_delivery/ctp_delivery.xlsx
+++ b/app/config/tables/ctp_delivery/forms/ctp_delivery/ctp_delivery.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="124">
   <si>
     <t>clause</t>
   </si>
@@ -74,9 +74,6 @@
     <t>required</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
     <t>async_assign_single_string</t>
   </si>
   <si>
@@ -113,22 +110,10 @@
     <t>valid</t>
   </si>
   <si>
-    <t>if</t>
-  </si>
-  <si>
     <t>yes_no</t>
   </si>
   <si>
     <t>try_again</t>
-  </si>
-  <si>
-    <t>goto item_scan</t>
-  </si>
-  <si>
-    <t>end if</t>
-  </si>
-  <si>
-    <t>else</t>
   </si>
   <si>
     <t>signature</t>
@@ -456,25 +441,10 @@
     <t>assigned_item_pack_code</t>
   </si>
   <si>
-    <t>This item pack is authorized. Please deliver.</t>
-  </si>
-  <si>
-    <t>Unauthorized Item Pack! Do not distribute this item pack.</t>
-  </si>
-  <si>
-    <t>data('assigned_item_pack_code')  !== data('item_pack_barcode')</t>
-  </si>
-  <si>
     <t>constraint</t>
   </si>
   <si>
-    <t>constraint_message</t>
-  </si>
-  <si>
-    <t>data('assigned_item_pack_code') === data('item_pack_barcode')</t>
-  </si>
-  <si>
-    <t>Item pack barcode must equal assigned item pack code.</t>
+    <t>data('assigned_item_pack_code') === data('item_pack_barcode') || data('assigned_item_pack_code') == '' || data('assigned_item_pack_code') == null || data('assigned_item_pack_code') == undefined</t>
   </si>
 </sst>
 </file>
@@ -665,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -685,7 +655,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1068,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1057,7 @@
     <col min="10" max="11" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1122,29 +1091,26 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="84" x14ac:dyDescent="0.25">
+      <c r="L1" s="43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="84" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G2" s="14"/>
-      <c r="H2" s="43" t="s">
-        <v>18</v>
+      <c r="H2" s="42" t="s">
+        <v>17</v>
       </c>
       <c r="I2"/>
       <c r="J2" s="1" t="b">
@@ -1153,21 +1119,21 @@
       </c>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="18"/>
+      <c r="H3" s="17"/>
       <c r="I3"/>
       <c r="J3" s="1" t="b">
         <f>TRUE()</f>
@@ -1175,120 +1141,28 @@
       </c>
       <c r="K3" s="10"/>
       <c r="L3" t="s">
-        <v>132</v>
-      </c>
-      <c r="M3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="11"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="E4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
       <c r="I4" s="17"/>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="1" t="b">
-        <f>TRUE()</f>
+      <c r="K4" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:13" ht="42" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="1:13" ht="24" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="18"/>
-      <c r="K9" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1307,34 +1181,34 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>115</v>
+      <c r="C1" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="A2" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:4" ht="240" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23" t="s">
-        <v>118</v>
+      <c r="A3" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1357,90 +1231,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="21" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="C2" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="D3" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="F3" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="G3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="23" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>47</v>
+      <c r="I3" s="22" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1464,54 +1338,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="28" t="s">
+      <c r="A2" s="18" t="s">
         <v>20</v>
       </c>
+      <c r="B2" s="27" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>30</v>
+      <c r="A3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>30</v>
+      <c r="A4" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
-        <v>21</v>
+      <c r="A5" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>26</v>
+      <c r="A6" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="C6" t="b">
         <f>TRUE()</f>
@@ -1535,60 +1409,60 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="34"/>
+    </row>
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="33">
+        <v>1</v>
+      </c>
+      <c r="C3" s="34"/>
+    </row>
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B4" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="34"/>
+    </row>
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="35"/>
-    </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="34">
-        <v>1</v>
-      </c>
-      <c r="C3" s="35"/>
-    </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="35"/>
-    </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="35"/>
+      <c r="B6" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1608,138 +1482,138 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1760,35 +1634,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>85</v>
+        <v>23</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>87</v>
+        <v>23</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1809,7 +1683,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -1817,18 +1691,18 @@
     </row>
     <row r="2" spans="1:2" ht="409" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>91</v>
+        <v>85</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>93</v>
+        <v>87</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1848,71 +1722,71 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="D2" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>95</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>87</v>
+        <v>47</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1932,67 +1806,67 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B5" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B6" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>108</v>
+      <c r="B7" s="22" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>21</v>
+      <c r="A8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add delivery translations for ctp. skip initialization for custom_distribution_reports.
</commit_message>
<xml_diff>
--- a/app/config/tables/ctp_delivery/forms/ctp_delivery/ctp_delivery.xlsx
+++ b/app/config/tables/ctp_delivery/forms/ctp_delivery/ctp_delivery.xlsx
@@ -9,19 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="5700" windowWidth="33300" windowHeight="19420" tabRatio="989"/>
+    <workbookView xWindow="19220" yWindow="4780" windowWidth="33300" windowHeight="19420" tabRatio="989" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="queries" sheetId="2" r:id="rId2"/>
     <sheet name="model" sheetId="3" r:id="rId3"/>
     <sheet name="settings" sheetId="4" r:id="rId4"/>
-    <sheet name="table_specific_translations" sheetId="5" r:id="rId5"/>
-    <sheet name="choices" sheetId="6" r:id="rId6"/>
-    <sheet name="calculates" sheetId="7" r:id="rId7"/>
-    <sheet name="properties" sheetId="8" r:id="rId8"/>
-    <sheet name="prompt_types" sheetId="9" r:id="rId9"/>
-    <sheet name="initial" sheetId="10" r:id="rId10"/>
+    <sheet name="choices" sheetId="6" r:id="rId5"/>
+    <sheet name="calculates" sheetId="7" r:id="rId6"/>
+    <sheet name="properties" sheetId="8" r:id="rId7"/>
+    <sheet name="prompt_types" sheetId="9" r:id="rId8"/>
+    <sheet name="initial" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="95">
   <si>
     <t>clause</t>
   </si>
@@ -80,18 +79,12 @@
     <t>get_barcoderanges</t>
   </si>
   <si>
-    <t>ranges</t>
-  </si>
-  <si>
     <t>get_itempack</t>
   </si>
   <si>
     <t>item_pack_name</t>
   </si>
   <si>
-    <t>summary</t>
-  </si>
-  <si>
     <t>item_scan</t>
   </si>
   <si>
@@ -107,9 +100,6 @@
     <t>Please confirm or update item pack barcode.</t>
   </si>
   <si>
-    <t>valid</t>
-  </si>
-  <si>
     <t>yes_no</t>
   </si>
   <si>
@@ -125,9 +115,6 @@
     <t>Sign for receipt of item</t>
   </si>
   <si>
-    <t>is_delivered</t>
-  </si>
-  <si>
     <t>query_name</t>
   </si>
   <si>
@@ -173,15 +160,6 @@
     <t>isSessionVariable</t>
   </si>
   <si>
-    <t>entitlement_id</t>
-  </si>
-  <si>
-    <t>delivery_id</t>
-  </si>
-  <si>
-    <t>delivery_time</t>
-  </si>
-  <si>
     <t>boolean</t>
   </si>
   <si>
@@ -207,72 +185,6 @@
   </si>
   <si>
     <t>instance_name</t>
-  </si>
-  <si>
-    <t>string_token</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>Delivery ID</t>
-  </si>
-  <si>
-    <t>date_time</t>
-  </si>
-  <si>
-    <t>Time of Delivery</t>
-  </si>
-  <si>
-    <t>delivery_site</t>
-  </si>
-  <si>
-    <t>Delivery Site</t>
-  </si>
-  <si>
-    <t>distributor</t>
-  </si>
-  <si>
-    <t>Distributor</t>
-  </si>
-  <si>
-    <t>scanned_item_pack</t>
-  </si>
-  <si>
-    <t>Scanned Item Pack</t>
-  </si>
-  <si>
-    <t>Entitlement ID</t>
-  </si>
-  <si>
-    <t>Is Delivered</t>
-  </si>
-  <si>
-    <t>Item Pack Barcode</t>
-  </si>
-  <si>
-    <t>Signature</t>
-  </si>
-  <si>
-    <t>Delivery Time</t>
-  </si>
-  <si>
-    <t>Receive Signature</t>
-  </si>
-  <si>
-    <t>Ranges</t>
-  </si>
-  <si>
-    <t>Try Again</t>
-  </si>
-  <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>Item Pack Name</t>
-  </si>
-  <si>
-    <t>Summary</t>
   </si>
   <si>
     <t>choice_list_name</t>
@@ -490,7 +402,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -533,14 +445,8 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -601,26 +507,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="hair">
         <color auto="1"/>
       </left>
@@ -635,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -681,15 +567,11 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1039,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1091,26 +973,26 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="43" t="s">
-        <v>122</v>
+      <c r="L1" s="39" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="84" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
       <c r="C2" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="G2" s="14"/>
-      <c r="H2" s="42" t="s">
-        <v>17</v>
+      <c r="H2" s="38" t="s">
+        <v>15</v>
       </c>
       <c r="I2"/>
       <c r="J2" s="1" t="b">
@@ -1123,14 +1005,14 @@
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>21</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="17"/>
@@ -1141,21 +1023,21 @@
       </c>
       <c r="K3" s="10"/>
       <c r="L3" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
@@ -1167,53 +1049,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:4" ht="240" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -1232,31 +1067,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="F1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
@@ -1264,57 +1099,57 @@
         <v>12</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>42</v>
-      </c>
       <c r="I2" s="22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="H3" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>42</v>
-      </c>
       <c r="I3" s="22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1325,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1345,49 +1180,41 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="b">
+      <c r="A5" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
@@ -1410,27 +1237,27 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B3" s="33">
         <v>1</v>
@@ -1439,28 +1266,28 @@
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C6" s="34"/>
     </row>
@@ -1472,197 +1299,45 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>82</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1671,7 +1346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1683,7 +1358,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -1691,18 +1366,18 @@
     </row>
     <row r="2" spans="1:2" ht="409" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1711,7 +1386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1722,71 +1397,71 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="A1" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>49</v>
+      <c r="E1" s="36" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>95</v>
+      <c r="A2" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>82</v>
+        <v>40</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1795,7 +1470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1807,7 +1482,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>2</v>
@@ -1815,50 +1490,50 @@
     </row>
     <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="48" x14ac:dyDescent="0.2">
@@ -1866,7 +1541,54 @@
         <v>11</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+    </row>
+    <row r="3" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>